<commit_message>
Added pure detection threshold
</commit_message>
<xml_diff>
--- a/summarized_results.xlsx
+++ b/summarized_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Subject</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>TNI</t>
+  </si>
+  <si>
+    <t>Tone detection threshold</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +196,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A23"/>
@@ -521,63 +527,66 @@
   <cols>
     <col min="1" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="7" t="s">
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="5" t="s">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
       <c r="B3" s="3">
         <v>0.3</v>
       </c>
@@ -605,26 +614,29 @@
       <c r="J3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -656,25 +668,28 @@
         <v>12.604166666666668</v>
       </c>
       <c r="K4" s="1">
+        <v>5</v>
+      </c>
+      <c r="L4" s="1">
         <v>-6.5241721398281172</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>4.3870056935114778</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>10.911177833339595</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>1.3091827622985193</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>1.3680463405048515</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>1.3386145514016854</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -706,25 +721,28 @@
         <v>30.390624999999993</v>
       </c>
       <c r="K5" s="1">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
         <v>-8.6170763591421942</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>14.635243008943799</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>23.252319368085992</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>0.85474316506418613</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>0.68941596213799206</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>0.77207956360108909</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -756,25 +774,28 @@
         <v>8.4895833333333286</v>
       </c>
       <c r="K6" s="1">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1">
         <v>-6.0314101857015023</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>8.1191141321194937</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>14.150524317820995</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>3.1866735799828314</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>3.494486237067544</v>
       </c>
-      <c r="P6" s="1">
+      <c r="Q6" s="1">
         <v>3.3405799085251875</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -806,25 +827,28 @@
         <v>18.046875</v>
       </c>
       <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
         <v>-7.5281977300381433</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>9.0678510997088591</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>16.596048829747001</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>0.55308877563091352</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>0.49093287827100118</v>
       </c>
-      <c r="P7" s="1">
+      <c r="Q7" s="1">
         <v>0.52201082695095735</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -856,25 +880,28 @@
         <v>12.65625</v>
       </c>
       <c r="K8" s="1">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1">
         <v>-13.191095751614851</v>
       </c>
-      <c r="L8" s="1">
+      <c r="M8" s="1">
         <v>4.2904002357909476</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>17.4814959874058</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>0.51219602933843988</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>0.48100390075500282</v>
       </c>
-      <c r="P8" s="1">
+      <c r="Q8" s="1">
         <v>0.49659996504672133</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -906,25 +933,28 @@
         <v>7.96875</v>
       </c>
       <c r="K9" s="1">
+        <v>5</v>
+      </c>
+      <c r="L9" s="1">
         <v>-4.0935296114894877</v>
       </c>
-      <c r="L9" s="1">
+      <c r="M9" s="1">
         <v>9.7302544131524957</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>13.823784024641984</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>1.8725127720662602</v>
       </c>
-      <c r="O9" s="1">
+      <c r="P9" s="1">
         <v>1.8365997053081746</v>
       </c>
-      <c r="P9" s="1">
+      <c r="Q9" s="1">
         <v>1.8545562386872174</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -956,25 +986,28 @@
         <v>9.1145833333333357</v>
       </c>
       <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1">
         <v>-4.4254085576937561</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>8.3707151136109204</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>12.796123671304677</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>2.3501748575983399</v>
       </c>
-      <c r="O10" s="1">
+      <c r="P10" s="1">
         <v>2.343713902964081</v>
       </c>
-      <c r="P10" s="1">
+      <c r="Q10" s="1">
         <v>2.3469443802812107</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1006,25 +1039,28 @@
         <v>9.4270833333333321</v>
       </c>
       <c r="K11" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="L11" s="1">
         <v>-4.2290178340189239</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>7.5884528960075865</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>11.81747073002651</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>0.97511992067126674</v>
       </c>
-      <c r="O11" s="1">
+      <c r="P11" s="1">
         <v>1.0589992602978024</v>
       </c>
-      <c r="P11" s="1">
+      <c r="Q11" s="1">
         <v>1.0170595904845345</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1056,25 +1092,28 @@
         <v>15.208333333333336</v>
       </c>
       <c r="K12" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="L12" s="1">
         <v>-7.1931886878545317</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>6.7875454578767851</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>13.980734145731317</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>1.9011998371514824</v>
       </c>
-      <c r="O12" s="1">
+      <c r="P12" s="1">
         <v>1.9835343982030653</v>
       </c>
-      <c r="P12" s="1">
+      <c r="Q12" s="1">
         <v>1.9423671176772739</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1106,25 +1145,28 @@
         <v>16.927083333333332</v>
       </c>
       <c r="K13" s="1">
+        <v>10</v>
+      </c>
+      <c r="L13" s="1">
         <v>-6.8087011445641057</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>6.2156088861906369</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>13.024310030754743</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>1.530657104613323</v>
       </c>
-      <c r="O13" s="1">
+      <c r="P13" s="1">
         <v>1.7730672828630769</v>
       </c>
-      <c r="P13" s="1">
+      <c r="Q13" s="1">
         <v>1.6518621937382001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1156,25 +1198,28 @@
         <v>30.807291666666668</v>
       </c>
       <c r="K14" s="1">
+        <v>5</v>
+      </c>
+      <c r="L14" s="1">
         <v>-7.671347522115413</v>
       </c>
-      <c r="L14" s="1">
+      <c r="M14" s="1">
         <v>13.311832022998788</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>20.983179545114201</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>0.46675006151358539</v>
       </c>
-      <c r="O14" s="1">
+      <c r="P14" s="1">
         <v>0.50497275526356789</v>
       </c>
-      <c r="P14" s="1">
+      <c r="Q14" s="1">
         <v>0.48586140838857661</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1206,25 +1251,28 @@
         <v>27.916666666666664</v>
       </c>
       <c r="K15" s="1">
+        <v>10</v>
+      </c>
+      <c r="L15" s="1">
         <v>-5.105633090884659</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>9.8444936500221054</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>14.950126740906764</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>0.81425345083130207</v>
       </c>
-      <c r="O15" s="1">
+      <c r="P15" s="1">
         <v>0.96165264183802823</v>
       </c>
-      <c r="P15" s="1">
+      <c r="Q15" s="1">
         <v>0.88795304633466521</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1256,25 +1304,28 @@
         <v>5</v>
       </c>
       <c r="K16" s="1">
+        <v>5</v>
+      </c>
+      <c r="L16" s="1">
         <v>3.8420831035665213</v>
       </c>
-      <c r="L16" s="1">
+      <c r="M16" s="1">
         <v>15.737125824234457</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>11.895042720667936</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>2.0061929101465186</v>
       </c>
-      <c r="O16" s="1">
+      <c r="P16" s="1">
         <v>2.1490994190599153</v>
       </c>
-      <c r="P16" s="1">
+      <c r="Q16" s="1">
         <v>2.0776461646032169</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1306,25 +1357,28 @@
         <v>17.864583333333332</v>
       </c>
       <c r="K17" s="1">
+        <v>5</v>
+      </c>
+      <c r="L17" s="1">
         <v>-6.2034505388778083</v>
       </c>
-      <c r="L17" s="1">
+      <c r="M17" s="1">
         <v>13.573758999503958</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>19.777209538381769</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
         <v>0.33130034685770188</v>
       </c>
-      <c r="O17" s="1">
+      <c r="P17" s="1">
         <v>0.32499640797153212</v>
       </c>
-      <c r="P17" s="1">
+      <c r="Q17" s="1">
         <v>0.328148377414617</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1356,25 +1410,28 @@
         <v>5.4427083333333357</v>
       </c>
       <c r="K18" s="1">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
         <v>-6.1077271232573906</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>4.988581668319048</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>11.096308791576439</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>2.0761153853843282</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>2.2330440475352487</v>
       </c>
-      <c r="P18" s="1">
+      <c r="Q18" s="1">
         <v>2.1545797164597884</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1406,25 +1463,28 @@
         <v>3.359375</v>
       </c>
       <c r="K19" s="1">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1">
         <v>10.330830161802737</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>14.288312996407537</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>3.9574828346048001</v>
       </c>
-      <c r="N19" s="1">
+      <c r="O19" s="1">
         <v>2.4299838877932372</v>
       </c>
-      <c r="O19" s="1">
+      <c r="P19" s="1">
         <v>2.3174272305342321</v>
       </c>
-      <c r="P19" s="1">
+      <c r="Q19" s="1">
         <v>2.3737055591637346</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1456,25 +1516,28 @@
         <v>9.9479166666666643</v>
       </c>
       <c r="K20" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="L20" s="1">
         <v>-2.3574450765257118</v>
       </c>
-      <c r="L20" s="1">
+      <c r="M20" s="1">
         <v>8.8819421400695013</v>
       </c>
-      <c r="M20" s="1">
+      <c r="N20" s="1">
         <v>11.239387216595214</v>
       </c>
-      <c r="N20" s="1">
+      <c r="O20" s="1">
         <v>1.7578282248173225</v>
       </c>
-      <c r="O20" s="1">
+      <c r="P20" s="1">
         <v>1.8098381676841031</v>
       </c>
-      <c r="P20" s="1">
+      <c r="Q20" s="1">
         <v>1.7838331962507128</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1506,25 +1569,28 @@
         <v>36.25</v>
       </c>
       <c r="K21" s="1">
+        <v>5</v>
+      </c>
+      <c r="L21" s="1">
         <v>-8.0591264830814637</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>15.548722104141934</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>23.607848587223398</v>
       </c>
-      <c r="N21" s="1">
+      <c r="O21" s="1">
         <v>0.27570359473627482</v>
       </c>
-      <c r="O21" s="1">
+      <c r="P21" s="1">
         <v>0.35044256081052233</v>
       </c>
-      <c r="P21" s="1">
+      <c r="Q21" s="1">
         <v>0.31307307777339854</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1556,25 +1622,28 @@
         <v>13.932291666666664</v>
       </c>
       <c r="K22" s="1">
+        <v>5</v>
+      </c>
+      <c r="L22" s="1">
         <v>-8.272642248650067</v>
       </c>
-      <c r="L22" s="1">
+      <c r="M22" s="1">
         <v>4.1398554727619414</v>
       </c>
-      <c r="M22" s="1">
+      <c r="N22" s="1">
         <v>12.412497721412009</v>
       </c>
-      <c r="N22" s="1">
+      <c r="O22" s="1">
         <v>0.53667588747335937</v>
       </c>
-      <c r="O22" s="1">
+      <c r="P22" s="1">
         <v>0.83059106489186418</v>
       </c>
-      <c r="P22" s="1">
+      <c r="Q22" s="1">
         <v>0.68363347618261172</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -1606,29 +1675,32 @@
         <v>17.96875</v>
       </c>
       <c r="K23" s="1">
+        <v>20</v>
+      </c>
+      <c r="L23" s="1">
         <v>7.5763960387704801</v>
       </c>
-      <c r="L23" s="1">
+      <c r="M23" s="1">
         <v>15.3846307990257</v>
       </c>
-      <c r="M23" s="1">
+      <c r="N23" s="1">
         <v>7.8082347602552202</v>
       </c>
-      <c r="N23" s="1">
+      <c r="O23" s="1">
         <v>1.7474048938377325</v>
       </c>
-      <c r="O23" s="1">
+      <c r="P23" s="1">
         <v>1.7804903643901442</v>
       </c>
-      <c r="P23" s="1">
+      <c r="Q23" s="1">
         <v>1.7639476291139382</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B1:J1"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="N1:P2"/>
+    <mergeCell ref="L1:N2"/>
+    <mergeCell ref="O1:Q2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>

</xml_diff>